<commit_message>
opened and saved again to fix format errors in test execution (weird)
</commit_message>
<xml_diff>
--- a/src/test/resources/exporter_example.xlsx
+++ b/src/test/resources/exporter_example.xlsx
@@ -256,18 +256,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -277,10 +277,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>